<commit_message>
Actualizo datos del Excel de línea de tiempo
</commit_message>
<xml_diff>
--- a/linea_tiempo_proyecto_eolico.xlsx
+++ b/linea_tiempo_proyecto_eolico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathan.diaz/Desktop/Linea de tiempo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E839C46-39F6-8640-9A25-621317333CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42EA93EC-E272-684B-A19F-579EABBEF0AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="199">
   <si>
     <t>ID</t>
   </si>
@@ -349,12 +349,6 @@
     <t>2025-07-05</t>
   </si>
   <si>
-    <t>2025-08-11</t>
-  </si>
-  <si>
-    <t>2025-09-06</t>
-  </si>
-  <si>
     <t>2025-09-09</t>
   </si>
   <si>
@@ -406,9 +400,6 @@
     <t>2025-08-05</t>
   </si>
   <si>
-    <t>2025-08-26</t>
-  </si>
-  <si>
     <t>2025-09-08</t>
   </si>
   <si>
@@ -623,6 +614,9 @@
   </si>
   <si>
     <t>Piloto 55kW</t>
+  </si>
+  <si>
+    <t>Reunión clientes potenciales</t>
   </si>
 </sst>
 </file>
@@ -692,12 +686,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1004,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J17" zoomScale="230" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1017,9 +1015,10 @@
     <col min="4" max="4" width="33.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="24.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1049,10 +1048,10 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -1074,7 +1073,7 @@
         <v>15</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -1102,14 +1101,14 @@
       <c r="H2" t="s">
         <v>99</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="J2" t="s">
-        <v>126</v>
+      <c r="J2" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="K2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L2">
         <v>100</v>
@@ -1118,16 +1117,16 @@
         <v>76</v>
       </c>
       <c r="N2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="P2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="Q2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -1155,14 +1154,14 @@
       <c r="H3" t="s">
         <v>99</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="J3" t="s">
-        <v>126</v>
+      <c r="J3" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="K3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L3">
         <v>100</v>
@@ -1171,16 +1170,16 @@
         <v>76</v>
       </c>
       <c r="N3" t="s">
+        <v>143</v>
+      </c>
+      <c r="O3" t="s">
         <v>146</v>
       </c>
-      <c r="O3" t="s">
-        <v>149</v>
-      </c>
       <c r="P3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="Q3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -1208,14 +1207,14 @@
       <c r="H4" t="s">
         <v>99</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="J4" t="s">
-        <v>126</v>
+      <c r="J4" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="K4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L4">
         <v>100</v>
@@ -1224,16 +1223,16 @@
         <v>76</v>
       </c>
       <c r="N4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="P4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="Q4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -1261,14 +1260,14 @@
       <c r="H5" t="s">
         <v>99</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="J5" t="s">
-        <v>127</v>
+      <c r="J5" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="K5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L5">
         <v>100</v>
@@ -1277,16 +1276,16 @@
         <v>76</v>
       </c>
       <c r="N5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O5" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="P5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="Q5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -1314,15 +1313,13 @@
       <c r="H6" t="s">
         <v>99</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="J6" t="s">
-        <v>127</v>
-      </c>
-      <c r="K6" t="s">
-        <v>127</v>
-      </c>
+      <c r="J6" s="3">
+        <v>45899</v>
+      </c>
+      <c r="K6" s="3"/>
       <c r="L6">
         <v>100</v>
       </c>
@@ -1330,16 +1327,16 @@
         <v>76</v>
       </c>
       <c r="N6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="P6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="Q6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -1367,12 +1364,13 @@
       <c r="H7" t="s">
         <v>100</v>
       </c>
-      <c r="I7" t="s">
-        <v>109</v>
-      </c>
-      <c r="J7" t="s">
-        <v>128</v>
-      </c>
+      <c r="I7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="J7" s="3">
+        <v>45895</v>
+      </c>
+      <c r="K7" s="3"/>
       <c r="L7">
         <v>60</v>
       </c>
@@ -1380,16 +1378,16 @@
         <v>4</v>
       </c>
       <c r="N7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="P7" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Q7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -1417,11 +1415,11 @@
       <c r="H8" t="s">
         <v>101</v>
       </c>
-      <c r="I8" t="s">
-        <v>110</v>
-      </c>
-      <c r="J8" t="s">
-        <v>129</v>
+      <c r="I8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1430,16 +1428,16 @@
         <v>6</v>
       </c>
       <c r="N8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="P8" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="Q8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -1467,11 +1465,11 @@
       <c r="H9" t="s">
         <v>101</v>
       </c>
-      <c r="I9" t="s">
-        <v>111</v>
-      </c>
-      <c r="J9" t="s">
-        <v>130</v>
+      <c r="I9" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1480,16 +1478,16 @@
         <v>7</v>
       </c>
       <c r="N9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="P9" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="Q9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -1517,11 +1515,11 @@
       <c r="H10" t="s">
         <v>101</v>
       </c>
-      <c r="I10" t="s">
-        <v>112</v>
-      </c>
-      <c r="J10" t="s">
-        <v>113</v>
+      <c r="I10" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1530,16 +1528,16 @@
         <v>8</v>
       </c>
       <c r="N10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="P10" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="Q10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -1567,29 +1565,29 @@
       <c r="H11" t="s">
         <v>101</v>
       </c>
-      <c r="I11" t="s">
-        <v>113</v>
-      </c>
-      <c r="J11" t="s">
-        <v>113</v>
+      <c r="I11" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="N11" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="O11" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="P11" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="Q11" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -1617,11 +1615,11 @@
       <c r="H12" t="s">
         <v>100</v>
       </c>
-      <c r="I12" t="s">
-        <v>114</v>
-      </c>
-      <c r="J12" t="s">
-        <v>131</v>
+      <c r="I12" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="L12">
         <v>80</v>
@@ -1630,16 +1628,16 @@
         <v>4</v>
       </c>
       <c r="N12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="P12" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="Q12" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -1667,11 +1665,11 @@
       <c r="H13" t="s">
         <v>102</v>
       </c>
-      <c r="I13" t="s">
-        <v>115</v>
-      </c>
-      <c r="J13" t="s">
-        <v>132</v>
+      <c r="I13" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -1680,16 +1678,16 @@
         <v>11</v>
       </c>
       <c r="N13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O13" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="P13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="Q13" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -1717,11 +1715,11 @@
       <c r="H14" t="s">
         <v>102</v>
       </c>
-      <c r="I14" t="s">
-        <v>116</v>
-      </c>
-      <c r="J14" t="s">
-        <v>117</v>
+      <c r="I14" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -1730,16 +1728,16 @@
         <v>12</v>
       </c>
       <c r="N14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="P14" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="Q14" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -1767,11 +1765,11 @@
       <c r="H15" t="s">
         <v>102</v>
       </c>
-      <c r="I15" t="s">
-        <v>117</v>
-      </c>
-      <c r="J15" t="s">
-        <v>133</v>
+      <c r="I15" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1780,16 +1778,16 @@
         <v>13</v>
       </c>
       <c r="N15" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O15" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="P15" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="Q15" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
@@ -1817,29 +1815,29 @@
       <c r="H16" t="s">
         <v>102</v>
       </c>
-      <c r="I16" t="s">
-        <v>118</v>
-      </c>
-      <c r="J16" t="s">
-        <v>134</v>
+      <c r="I16" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="N16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="P16" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="Q16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
@@ -1867,11 +1865,11 @@
       <c r="H17" t="s">
         <v>102</v>
       </c>
-      <c r="I17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J17" t="s">
-        <v>135</v>
+      <c r="I17" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -1880,16 +1878,16 @@
         <v>15</v>
       </c>
       <c r="N17" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O17" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="P17" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="Q17" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
@@ -1917,11 +1915,11 @@
       <c r="H18" t="s">
         <v>102</v>
       </c>
-      <c r="I18" t="s">
-        <v>120</v>
-      </c>
-      <c r="J18" t="s">
-        <v>136</v>
+      <c r="I18" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1930,16 +1928,16 @@
         <v>4</v>
       </c>
       <c r="N18" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O18" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="P18" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="Q18" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
@@ -1967,29 +1965,29 @@
       <c r="H19" t="s">
         <v>102</v>
       </c>
-      <c r="I19" t="s">
-        <v>121</v>
-      </c>
-      <c r="J19" t="s">
-        <v>137</v>
+      <c r="I19" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="N19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O19" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="P19" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="Q19" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
@@ -2017,11 +2015,11 @@
       <c r="H20" t="s">
         <v>102</v>
       </c>
-      <c r="I20" t="s">
-        <v>122</v>
-      </c>
-      <c r="J20" t="s">
-        <v>138</v>
+      <c r="I20" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -2030,16 +2028,16 @@
         <v>18</v>
       </c>
       <c r="N20" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O20" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="P20" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="Q20" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
@@ -2067,11 +2065,11 @@
       <c r="H21" t="s">
         <v>102</v>
       </c>
-      <c r="I21" t="s">
-        <v>123</v>
-      </c>
-      <c r="J21" t="s">
-        <v>123</v>
+      <c r="I21" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -2080,16 +2078,16 @@
         <v>19</v>
       </c>
       <c r="N21" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="O21" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="P21" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="Q21" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
@@ -2117,11 +2115,11 @@
       <c r="H22" t="s">
         <v>102</v>
       </c>
-      <c r="I22" t="s">
-        <v>124</v>
-      </c>
-      <c r="J22" t="s">
-        <v>139</v>
+      <c r="I22" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -2130,16 +2128,16 @@
         <v>19</v>
       </c>
       <c r="N22" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O22" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="P22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="Q22" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
@@ -2167,11 +2165,11 @@
       <c r="H23" t="s">
         <v>103</v>
       </c>
-      <c r="I23" t="s">
-        <v>124</v>
-      </c>
-      <c r="J23" t="s">
-        <v>139</v>
+      <c r="I23" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -2180,16 +2178,16 @@
         <v>21</v>
       </c>
       <c r="N23" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O23" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="P23" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="Q23" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
@@ -2217,11 +2215,11 @@
       <c r="H24" t="s">
         <v>102</v>
       </c>
-      <c r="I24" t="s">
-        <v>123</v>
-      </c>
-      <c r="J24" t="s">
-        <v>140</v>
+      <c r="I24" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -2230,16 +2228,16 @@
         <v>20</v>
       </c>
       <c r="N24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O24" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="P24" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="Q24" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
@@ -2267,11 +2265,11 @@
       <c r="H25" t="s">
         <v>101</v>
       </c>
-      <c r="I25" t="s">
-        <v>124</v>
-      </c>
-      <c r="J25" t="s">
-        <v>141</v>
+      <c r="I25" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>138</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -2280,16 +2278,16 @@
         <v>23</v>
       </c>
       <c r="N25" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O25" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="P25" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q25" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
@@ -2317,11 +2315,11 @@
       <c r="H26" t="s">
         <v>101</v>
       </c>
-      <c r="I26" t="s">
-        <v>125</v>
-      </c>
-      <c r="J26" t="s">
-        <v>142</v>
+      <c r="I26" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -2330,16 +2328,66 @@
         <v>24</v>
       </c>
       <c r="N26" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="O26" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="P26" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q26" t="s">
         <v>197</v>
       </c>
-      <c r="Q26" t="s">
-        <v>200</v>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" t="s">
+        <v>198</v>
+      </c>
+      <c r="E27" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" t="s">
+        <v>102</v>
+      </c>
+      <c r="I27" s="3">
+        <v>45991</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>20</v>
+      </c>
+      <c r="N27" t="s">
+        <v>143</v>
+      </c>
+      <c r="O27" t="s">
+        <v>167</v>
+      </c>
+      <c r="P27" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>